<commit_message>
Improve the description and text based on the new information
</commit_message>
<xml_diff>
--- a/output/output_cholensky.xlsx
+++ b/output/output_cholensky.xlsx
@@ -20,16 +20,16 @@
     <t xml:space="preserve"/>
   </si>
   <si>
+    <t xml:space="preserve">OS mito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OS caba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PFS mito</t>
+  </si>
+  <si>
     <t xml:space="preserve">PFS caba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PFS mito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OS caba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OS mito</t>
   </si>
   <si>
     <t xml:space="preserve">exponential</t>
@@ -407,16 +407,16 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
+        <v>0.0577563498373389</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.0577539039418792</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0577585414814766</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.0577589819280178</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.0577585414814766</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.0577539039418792</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.0577563498373389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Identify error in function
The data structured used in the function had a different format. Therefore, we were not using the correct data. This is now updated
</commit_message>
<xml_diff>
--- a/output/output_cholensky.xlsx
+++ b/output/output_cholensky.xlsx
@@ -410,13 +410,13 @@
         <v>0.0577563498373389</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0577539039418792</v>
+        <v>0.0606465275779165</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0577585414814766</v>
+        <v>0.0527586331715868</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0577589819280178</v>
+        <v>0.0540637390173801</v>
       </c>
     </row>
   </sheetData>
@@ -457,7 +457,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0348924203928159</v>
+        <v>0.0589862330212438</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -468,10 +468,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.00625134536889363</v>
+        <v>-0.0113584882966721</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0479781450907104</v>
+        <v>0.0452961847902155</v>
       </c>
     </row>
     <row r="6">
@@ -495,7 +495,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0349632862897667</v>
+        <v>0.0619592603432408</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -506,10 +506,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.00593965997401846</v>
+        <v>-0.0128179425420927</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0481065976060797</v>
+        <v>0.0406511128175405</v>
       </c>
     </row>
     <row r="11">
@@ -533,7 +533,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0384466674668481</v>
+        <v>0.0405087071958447</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -544,10 +544,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="n">
-        <v>-0.00344171149344275</v>
+        <v>0.00275245948638132</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0483804502837504</v>
+        <v>0.0525507587379983</v>
       </c>
     </row>
     <row r="16">
@@ -626,7 +626,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0424383448345619</v>
+        <v>0.0617677799350474</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -637,10 +637,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0034910938462956</v>
+        <v>-0.0019259391554576</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0434930040119971</v>
+        <v>0.0445890580851386</v>
       </c>
     </row>
     <row r="6">
@@ -664,7 +664,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0425549694372227</v>
+        <v>0.0562954952310476</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -675,10 +675,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.00365049346203166</v>
+        <v>-0.00309717690119501</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0435211218851646</v>
+        <v>0.042669435266441</v>
       </c>
     </row>
     <row r="11">
@@ -702,7 +702,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0450291883081754</v>
+        <v>0.0495164494110894</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -713,10 +713,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="n">
-        <v>0.00498890657306087</v>
+        <v>0.00854800860377524</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0437949087084597</v>
+        <v>0.0460967621500772</v>
       </c>
     </row>
     <row r="16">
@@ -795,7 +795,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0401340568325777</v>
+        <v>0.0640912155632968</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
@@ -806,10 +806,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>0.000194083209764814</v>
+        <v>-0.000982529676603334</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0493276258765295</v>
+        <v>0.0487655237850791</v>
       </c>
     </row>
     <row r="6">
@@ -833,7 +833,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0402377671742021</v>
+        <v>0.0567696803186672</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -844,10 +844,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.000322140315558571</v>
+        <v>0.00141827357831441</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0493370924535617</v>
+        <v>0.0480355167606601</v>
       </c>
     </row>
     <row r="11">
@@ -871,7 +871,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0425470059622097</v>
+        <v>0.0458233048611451</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -882,10 +882,10 @@
         <v>8</v>
       </c>
       <c r="B14" t="n">
-        <v>0.00189830735243867</v>
+        <v>0.00436994056411851</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0494343385542332</v>
+        <v>0.052409913253889</v>
       </c>
     </row>
     <row r="16">

</xml_diff>

<commit_message>
Rename the values with a dash rather then space
</commit_message>
<xml_diff>
--- a/output/output_cholensky.xlsx
+++ b/output/output_cholensky.xlsx
@@ -20,22 +20,22 @@
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">OS mito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OS caba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PFS mito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PFS caba</t>
+    <t xml:space="preserve">OS_mito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OS_caba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PFS_mito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PFS_caba</t>
   </si>
   <si>
     <t xml:space="preserve">exponential</t>
   </si>
   <si>
-    <t xml:space="preserve">Model: PFS caba</t>
+    <t xml:space="preserve">Model: PFS_caba</t>
   </si>
   <si>
     <t xml:space="preserve">(Intercept)</t>
@@ -44,13 +44,13 @@
     <t xml:space="preserve">Log(scale)</t>
   </si>
   <si>
-    <t xml:space="preserve">Model: PFS mito</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model: OS caba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Model: OS mito</t>
+    <t xml:space="preserve">Model: PFS_mito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model: OS_caba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Model: OS_mito</t>
   </si>
 </sst>
 </file>

</xml_diff>